<commit_message>
rekap pdu taruna 2021-2
</commit_message>
<xml_diff>
--- a/27. TARUNA 2021-2 E(K_1) N(K_2) T(K_3)/UKURAN.xlsx
+++ b/27. TARUNA 2021-2 E(K_1) N(K_2) T(K_3)/UKURAN.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mapan\progress\27. TARUNA 2021-2 E(K_1) N(K_2) T(K_3)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F86B81F-7753-42B8-A4FA-23EB2A717A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416D0680-CE65-410D-936B-A66229BBA8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D0EA34A-D090-461B-B73E-10F00D55D97B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{8D0EA34A-D090-461B-B73E-10F00D55D97B}"/>
   </bookViews>
   <sheets>
     <sheet name="SEMUA" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="rekap" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SEMUA!$A$1:$Z$255</definedName>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1315" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="566">
   <si>
     <t>ARUM PAMBUDININGTYAS</t>
   </si>
@@ -1719,6 +1720,15 @@
   </si>
   <si>
     <t>D-III TEKNIKA REGULER</t>
+  </si>
+  <si>
+    <t>topi</t>
+  </si>
+  <si>
+    <t>pria</t>
+  </si>
+  <si>
+    <t>PESAN</t>
   </si>
 </sst>
 </file>
@@ -2304,12 +2314,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0593BD49-364B-49CF-AB09-840279B88535}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:Z535"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X261" sqref="X261"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A237" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2:E255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2407,7 +2416,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="23.25" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="23.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>208</v>
       </c>
@@ -2481,7 +2490,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>209</v>
       </c>
@@ -2555,7 +2564,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>210</v>
       </c>
@@ -2629,7 +2638,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>211</v>
       </c>
@@ -2703,7 +2712,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="23.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>212</v>
       </c>
@@ -2777,7 +2786,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>213</v>
       </c>
@@ -2851,7 +2860,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>214</v>
       </c>
@@ -2925,7 +2934,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>215</v>
       </c>
@@ -2999,7 +3008,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>216</v>
       </c>
@@ -3073,7 +3082,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>217</v>
       </c>
@@ -3147,7 +3156,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>218</v>
       </c>
@@ -3369,7 +3378,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>221</v>
       </c>
@@ -3443,7 +3452,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>222</v>
       </c>
@@ -3517,7 +3526,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>223</v>
       </c>
@@ -3591,7 +3600,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>224</v>
       </c>
@@ -3665,7 +3674,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>225</v>
       </c>
@@ -3813,7 +3822,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>227</v>
       </c>
@@ -3887,7 +3896,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>228</v>
       </c>
@@ -3961,7 +3970,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>229</v>
       </c>
@@ -4035,7 +4044,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="24" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>230</v>
       </c>
@@ -4109,7 +4118,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>231</v>
       </c>
@@ -4183,7 +4192,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="26" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>232</v>
       </c>
@@ -4257,7 +4266,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="27" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>233</v>
       </c>
@@ -4331,7 +4340,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>234</v>
       </c>
@@ -4553,7 +4562,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="31" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>237</v>
       </c>
@@ -4701,7 +4710,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>239</v>
       </c>
@@ -4775,7 +4784,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>240</v>
       </c>
@@ -4849,7 +4858,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="35" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>241</v>
       </c>
@@ -4923,7 +4932,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="36" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>242</v>
       </c>
@@ -5145,7 +5154,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="39" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>245</v>
       </c>
@@ -5219,7 +5228,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="40" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>246</v>
       </c>
@@ -5293,7 +5302,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="41" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>247</v>
       </c>
@@ -5367,7 +5376,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="42" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>248</v>
       </c>
@@ -5441,7 +5450,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="43" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>249</v>
       </c>
@@ -5515,7 +5524,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="44" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>250</v>
       </c>
@@ -5589,7 +5598,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="45" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>251</v>
       </c>
@@ -5663,7 +5672,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="46" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>252</v>
       </c>
@@ -5737,7 +5746,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="47" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>253</v>
       </c>
@@ -5811,7 +5820,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="48" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>254</v>
       </c>
@@ -5885,7 +5894,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="49" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>255</v>
       </c>
@@ -5959,7 +5968,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="50" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>256</v>
       </c>
@@ -6033,7 +6042,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="51" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
         <v>257</v>
       </c>
@@ -6107,7 +6116,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="52" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>258</v>
       </c>
@@ -6181,7 +6190,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="53" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>259</v>
       </c>
@@ -6255,7 +6264,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="54" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>260</v>
       </c>
@@ -6329,7 +6338,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="55" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>261</v>
       </c>
@@ -6403,7 +6412,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="56" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>262</v>
       </c>
@@ -6477,7 +6486,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="57" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>263</v>
       </c>
@@ -6699,7 +6708,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="60" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>266</v>
       </c>
@@ -6773,7 +6782,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="61" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>267</v>
       </c>
@@ -6847,7 +6856,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="62" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>268</v>
       </c>
@@ -6873,7 +6882,7 @@
       <c r="O62" s="20"/>
       <c r="P62" s="21"/>
     </row>
-    <row r="63" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
         <v>269</v>
       </c>
@@ -6899,7 +6908,7 @@
       <c r="O63" s="22"/>
       <c r="P63" s="23"/>
     </row>
-    <row r="64" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>270</v>
       </c>
@@ -6973,7 +6982,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="65" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
         <v>271</v>
       </c>
@@ -7047,7 +7056,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="66" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>272</v>
       </c>
@@ -7121,7 +7130,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="67" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
         <v>273</v>
       </c>
@@ -7269,7 +7278,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="69" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
         <v>275</v>
       </c>
@@ -7417,7 +7426,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="71" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
         <v>277</v>
       </c>
@@ -7491,7 +7500,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="72" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>278</v>
       </c>
@@ -7565,7 +7574,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="73" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
         <v>279</v>
       </c>
@@ -7639,7 +7648,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="74" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>280</v>
       </c>
@@ -7713,7 +7722,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="75" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
         <v>281</v>
       </c>
@@ -7787,7 +7796,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="76" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>282</v>
       </c>
@@ -7861,7 +7870,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="77" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
         <v>283</v>
       </c>
@@ -7935,7 +7944,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="78" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>284</v>
       </c>
@@ -8009,7 +8018,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="79" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
         <v>285</v>
       </c>
@@ -8083,7 +8092,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="80" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>286</v>
       </c>
@@ -8157,7 +8166,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="81" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
         <v>287</v>
       </c>
@@ -8231,7 +8240,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="82" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>288</v>
       </c>
@@ -8305,7 +8314,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="83" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
         <v>289</v>
       </c>
@@ -8379,7 +8388,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="84" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>290</v>
       </c>
@@ -8453,7 +8462,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="85" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
         <v>291</v>
       </c>
@@ -8527,7 +8536,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="86" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>292</v>
       </c>
@@ -8675,7 +8684,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="88" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>294</v>
       </c>
@@ -8749,7 +8758,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="89" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="s">
         <v>295</v>
       </c>
@@ -8823,7 +8832,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="90" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>296</v>
       </c>
@@ -8897,7 +8906,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="91" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="s">
         <v>297</v>
       </c>
@@ -8971,7 +8980,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="92" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>298</v>
       </c>
@@ -8997,7 +9006,7 @@
       <c r="O92" s="20"/>
       <c r="P92" s="21"/>
     </row>
-    <row r="93" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="s">
         <v>299</v>
       </c>
@@ -9145,7 +9154,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="95" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="12" t="s">
         <v>301</v>
       </c>
@@ -9219,7 +9228,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="96" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>302</v>
       </c>
@@ -9441,7 +9450,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="99" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="12" t="s">
         <v>305</v>
       </c>
@@ -9515,7 +9524,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="100" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>306</v>
       </c>
@@ -9589,7 +9598,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="101" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="s">
         <v>307</v>
       </c>
@@ -9663,7 +9672,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="102" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>308</v>
       </c>
@@ -9737,7 +9746,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="103" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="12" t="s">
         <v>309</v>
       </c>
@@ -9811,7 +9820,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="104" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>310</v>
       </c>
@@ -9959,7 +9968,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="106" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>312</v>
       </c>
@@ -10033,7 +10042,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="107" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="12" t="s">
         <v>313</v>
       </c>
@@ -10107,7 +10116,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="108" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>314</v>
       </c>
@@ -10181,7 +10190,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="109" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="12" t="s">
         <v>315</v>
       </c>
@@ -10255,7 +10264,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="110" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>316</v>
       </c>
@@ -10329,7 +10338,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="111" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="12" t="s">
         <v>317</v>
       </c>
@@ -10403,7 +10412,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="112" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>318</v>
       </c>
@@ -10551,7 +10560,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="114" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>320</v>
       </c>
@@ -10625,7 +10634,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="115" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="12" t="s">
         <v>321</v>
       </c>
@@ -10699,7 +10708,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="116" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>322</v>
       </c>
@@ -10773,7 +10782,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="117" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="12" t="s">
         <v>323</v>
       </c>
@@ -10847,7 +10856,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="118" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>324</v>
       </c>
@@ -10873,7 +10882,7 @@
       <c r="O118" s="20"/>
       <c r="P118" s="21"/>
     </row>
-    <row r="119" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="12" t="s">
         <v>325</v>
       </c>
@@ -10947,7 +10956,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="120" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>326</v>
       </c>
@@ -11021,7 +11030,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="121" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="12" t="s">
         <v>327</v>
       </c>
@@ -11243,7 +11252,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="124" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>330</v>
       </c>
@@ -11317,7 +11326,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="125" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="12" t="s">
         <v>331</v>
       </c>
@@ -11391,7 +11400,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="126" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>332</v>
       </c>
@@ -11465,7 +11474,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="127" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="12" t="s">
         <v>333</v>
       </c>
@@ -11604,7 +11613,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="129" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="12" t="s">
         <v>335</v>
       </c>
@@ -11678,7 +11687,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="130" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>336</v>
       </c>
@@ -11817,7 +11826,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="132" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>338</v>
       </c>
@@ -11891,7 +11900,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="133" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="12" t="s">
         <v>339</v>
       </c>
@@ -11917,7 +11926,7 @@
       <c r="O133" s="22"/>
       <c r="P133" s="23"/>
     </row>
-    <row r="134" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>340</v>
       </c>
@@ -11991,7 +12000,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="135" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="12" t="s">
         <v>341</v>
       </c>
@@ -12065,7 +12074,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="136" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>342</v>
       </c>
@@ -12139,7 +12148,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="137" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="12" t="s">
         <v>343</v>
       </c>
@@ -12213,7 +12222,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="138" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>344</v>
       </c>
@@ -12435,7 +12444,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="141" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="12" t="s">
         <v>347</v>
       </c>
@@ -12583,7 +12592,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="143" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="12" t="s">
         <v>349</v>
       </c>
@@ -12657,7 +12666,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="144" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>350</v>
       </c>
@@ -12731,7 +12740,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="145" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="12" t="s">
         <v>351</v>
       </c>
@@ -12805,7 +12814,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="146" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>352</v>
       </c>
@@ -12879,7 +12888,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="147" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="12" t="s">
         <v>353</v>
       </c>
@@ -12953,7 +12962,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="148" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>354</v>
       </c>
@@ -13027,7 +13036,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="149" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="12" t="s">
         <v>355</v>
       </c>
@@ -13101,7 +13110,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="150" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>356</v>
       </c>
@@ -13175,7 +13184,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="151" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="12" t="s">
         <v>357</v>
       </c>
@@ -13249,7 +13258,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="152" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>358</v>
       </c>
@@ -13275,7 +13284,7 @@
       <c r="O152" s="20"/>
       <c r="P152" s="21"/>
     </row>
-    <row r="153" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="12" t="s">
         <v>359</v>
       </c>
@@ -13349,7 +13358,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="154" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="10" t="s">
         <v>360</v>
       </c>
@@ -13423,7 +13432,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="155" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="12" t="s">
         <v>361</v>
       </c>
@@ -13497,7 +13506,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="10" t="s">
         <v>362</v>
       </c>
@@ -13571,7 +13580,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="157" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="12" t="s">
         <v>363</v>
       </c>
@@ -13645,7 +13654,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="158" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="10" t="s">
         <v>364</v>
       </c>
@@ -13719,7 +13728,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="159" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="12" t="s">
         <v>365</v>
       </c>
@@ -13793,7 +13802,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="160" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="10" t="s">
         <v>366</v>
       </c>
@@ -13867,7 +13876,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="161" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="12" t="s">
         <v>367</v>
       </c>
@@ -13941,7 +13950,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="162" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="10" t="s">
         <v>368</v>
       </c>
@@ -14015,7 +14024,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="163" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="12" t="s">
         <v>369</v>
       </c>
@@ -14089,7 +14098,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="164" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="10" t="s">
         <v>370</v>
       </c>
@@ -14163,7 +14172,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="165" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="12" t="s">
         <v>371</v>
       </c>
@@ -14237,7 +14246,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="166" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="10" t="s">
         <v>372</v>
       </c>
@@ -14311,7 +14320,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="167" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="12" t="s">
         <v>373</v>
       </c>
@@ -14385,7 +14394,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="168" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="10" t="s">
         <v>374</v>
       </c>
@@ -14459,7 +14468,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="169" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="12" t="s">
         <v>375</v>
       </c>
@@ -14533,7 +14542,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="170" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="10" t="s">
         <v>376</v>
       </c>
@@ -14607,7 +14616,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="171" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="12" t="s">
         <v>377</v>
       </c>
@@ -14681,7 +14690,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="172" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="10" t="s">
         <v>378</v>
       </c>
@@ -14755,7 +14764,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="173" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="12" t="s">
         <v>379</v>
       </c>
@@ -14829,7 +14838,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="174" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="10" t="s">
         <v>380</v>
       </c>
@@ -14903,7 +14912,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="175" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="12" t="s">
         <v>381</v>
       </c>
@@ -15051,7 +15060,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="177" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="12" t="s">
         <v>383</v>
       </c>
@@ -15125,7 +15134,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="178" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="10" t="s">
         <v>384</v>
       </c>
@@ -15199,7 +15208,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="179" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="12" t="s">
         <v>385</v>
       </c>
@@ -15273,7 +15282,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="180" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="10" t="s">
         <v>386</v>
       </c>
@@ -15347,7 +15356,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="181" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="12" t="s">
         <v>387</v>
       </c>
@@ -15421,7 +15430,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="182" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="10" t="s">
         <v>388</v>
       </c>
@@ -15495,7 +15504,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="183" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="12" t="s">
         <v>389</v>
       </c>
@@ -15569,7 +15578,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="184" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="10" t="s">
         <v>390</v>
       </c>
@@ -15643,7 +15652,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="185" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="12" t="s">
         <v>391</v>
       </c>
@@ -15717,7 +15726,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="186" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="10" t="s">
         <v>392</v>
       </c>
@@ -15791,7 +15800,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="187" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="12" t="s">
         <v>393</v>
       </c>
@@ -15865,7 +15874,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="188" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="10" t="s">
         <v>394</v>
       </c>
@@ -15939,7 +15948,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="189" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="12" t="s">
         <v>395</v>
       </c>
@@ -16013,7 +16022,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="190" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="10" t="s">
         <v>396</v>
       </c>
@@ -16087,7 +16096,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="191" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="12" t="s">
         <v>397</v>
       </c>
@@ -16161,7 +16170,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="192" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="10" t="s">
         <v>398</v>
       </c>
@@ -16235,7 +16244,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="193" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="12" t="s">
         <v>399</v>
       </c>
@@ -16309,7 +16318,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="194" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="10" t="s">
         <v>400</v>
       </c>
@@ -16383,7 +16392,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="195" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="12" t="s">
         <v>401</v>
       </c>
@@ -16457,7 +16466,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="196" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="10" t="s">
         <v>402</v>
       </c>
@@ -16531,7 +16540,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="197" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="12" t="s">
         <v>403</v>
       </c>
@@ -16605,7 +16614,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="198" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="10" t="s">
         <v>404</v>
       </c>
@@ -16679,7 +16688,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="199" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="12" t="s">
         <v>405</v>
       </c>
@@ -16753,7 +16762,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="200" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="10" t="s">
         <v>406</v>
       </c>
@@ -16827,7 +16836,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="201" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="12" t="s">
         <v>407</v>
       </c>
@@ -16901,7 +16910,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="202" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="10" t="s">
         <v>408</v>
       </c>
@@ -16975,7 +16984,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="203" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="12" t="s">
         <v>409</v>
       </c>
@@ -17049,7 +17058,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="204" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="10" t="s">
         <v>410</v>
       </c>
@@ -17123,7 +17132,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="205" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="12" t="s">
         <v>411</v>
       </c>
@@ -17197,7 +17206,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="206" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="10" t="s">
         <v>412</v>
       </c>
@@ -17271,7 +17280,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="207" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="12" t="s">
         <v>413</v>
       </c>
@@ -17345,7 +17354,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="208" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="10" t="s">
         <v>414</v>
       </c>
@@ -17419,7 +17428,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="12" t="s">
         <v>415</v>
       </c>
@@ -17493,7 +17502,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="210" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="10" t="s">
         <v>416</v>
       </c>
@@ -17567,7 +17576,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="211" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="12" t="s">
         <v>417</v>
       </c>
@@ -17641,7 +17650,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="212" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="10" t="s">
         <v>418</v>
       </c>
@@ -17715,7 +17724,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="213" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="12" t="s">
         <v>419</v>
       </c>
@@ -17789,7 +17798,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="214" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="10" t="s">
         <v>420</v>
       </c>
@@ -17863,7 +17872,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="215" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="12" t="s">
         <v>421</v>
       </c>
@@ -17937,7 +17946,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="216" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="10" t="s">
         <v>422</v>
       </c>
@@ -18011,7 +18020,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="217" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="12" t="s">
         <v>423</v>
       </c>
@@ -18085,7 +18094,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="218" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="10" t="s">
         <v>424</v>
       </c>
@@ -18159,7 +18168,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="219" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="12" t="s">
         <v>425</v>
       </c>
@@ -18233,7 +18242,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="220" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="10" t="s">
         <v>426</v>
       </c>
@@ -18307,7 +18316,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="221" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="12" t="s">
         <v>427</v>
       </c>
@@ -18381,7 +18390,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="222" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="10" t="s">
         <v>428</v>
       </c>
@@ -18455,7 +18464,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="223" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="12" t="s">
         <v>429</v>
       </c>
@@ -18529,7 +18538,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="224" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="10" t="s">
         <v>430</v>
       </c>
@@ -18603,7 +18612,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="225" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="12" t="s">
         <v>431</v>
       </c>
@@ -18677,7 +18686,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="226" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="10" t="s">
         <v>432</v>
       </c>
@@ -18751,7 +18760,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="227" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="12" t="s">
         <v>433</v>
       </c>
@@ -18825,7 +18834,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="228" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="10" t="s">
         <v>434</v>
       </c>
@@ -18899,7 +18908,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="229" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="12" t="s">
         <v>435</v>
       </c>
@@ -18973,7 +18982,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="230" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="10" t="s">
         <v>436</v>
       </c>
@@ -19047,7 +19056,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="231" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="12" t="s">
         <v>437</v>
       </c>
@@ -19121,7 +19130,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="232" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="10" t="s">
         <v>438</v>
       </c>
@@ -19195,7 +19204,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="233" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="12" t="s">
         <v>439</v>
       </c>
@@ -19269,7 +19278,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="234" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="10" t="s">
         <v>440</v>
       </c>
@@ -19343,7 +19352,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="235" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="12" t="s">
         <v>441</v>
       </c>
@@ -19369,7 +19378,7 @@
       <c r="O235" s="22"/>
       <c r="P235" s="23"/>
     </row>
-    <row r="236" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="10" t="s">
         <v>442</v>
       </c>
@@ -19443,7 +19452,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="237" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="12" t="s">
         <v>443</v>
       </c>
@@ -19517,7 +19526,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="238" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="10" t="s">
         <v>444</v>
       </c>
@@ -19591,7 +19600,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="239" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="12" t="s">
         <v>445</v>
       </c>
@@ -19665,7 +19674,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="240" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="10" t="s">
         <v>446</v>
       </c>
@@ -19739,7 +19748,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="241" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="12" t="s">
         <v>447</v>
       </c>
@@ -19813,7 +19822,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="242" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="10" t="s">
         <v>448</v>
       </c>
@@ -19887,7 +19896,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="243" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="12" t="s">
         <v>449</v>
       </c>
@@ -19961,7 +19970,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="244" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="10" t="s">
         <v>450</v>
       </c>
@@ -20035,7 +20044,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="245" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="12" t="s">
         <v>451</v>
       </c>
@@ -20109,7 +20118,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="246" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="10" t="s">
         <v>452</v>
       </c>
@@ -20183,7 +20192,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="247" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="12" t="s">
         <v>453</v>
       </c>
@@ -20257,7 +20266,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="248" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="10" t="s">
         <v>454</v>
       </c>
@@ -20331,7 +20340,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="249" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="12" t="s">
         <v>455</v>
       </c>
@@ -20405,7 +20414,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="250" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="10" t="s">
         <v>456</v>
       </c>
@@ -20479,7 +20488,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="251" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="12" t="s">
         <v>457</v>
       </c>
@@ -20553,7 +20562,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="252" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="10" t="s">
         <v>458</v>
       </c>
@@ -20627,7 +20636,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="253" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="12" t="s">
         <v>459</v>
       </c>
@@ -20701,7 +20710,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="254" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="10" t="s">
         <v>460</v>
       </c>
@@ -20775,7 +20784,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="255" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="12" t="s">
         <v>461</v>
       </c>
@@ -25638,13 +25647,6 @@
       <c r="L535" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z255" xr:uid="{0593BD49-364B-49CF-AB09-840279B88535}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="WANITA"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.43307086614173229" right="0.11811023622047245" top="0.51181102362204722" bottom="0.19685039370078741" header="0.19685039370078741" footer="0.11811023622047245"/>
@@ -25656,11 +25658,217 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F0D2B3-E601-4F53-A109-AB1348321EE0}">
+  <dimension ref="B2:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>563</v>
+      </c>
+      <c r="C2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E2" t="s">
+        <v>565</v>
+      </c>
+      <c r="G2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="18">
+        <v>53</v>
+      </c>
+      <c r="C3">
+        <f>COUNTIFS(SEMUA!$F$1:$F$255,rekap!$C$2,SEMUA!$E$1:$E$255,rekap!B3)</f>
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <f>COUNTIFS(SEMUA!$F$1:$F$255,rekap!$D$2,SEMUA!$E$1:$E$255,rekap!B3)</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>11</v>
+      </c>
+      <c r="G3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="15">
+        <v>54</v>
+      </c>
+      <c r="C4">
+        <f>COUNTIFS(SEMUA!$F$1:$F$255,rekap!$C$2,SEMUA!$E$1:$E$255,rekap!B4)</f>
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <f>COUNTIFS(SEMUA!$F$1:$F$255,rekap!$D$2,SEMUA!$E$1:$E$255,rekap!B4)</f>
+        <v>6</v>
+      </c>
+      <c r="E4">
+        <v>22</v>
+      </c>
+      <c r="G4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="14">
+        <v>55</v>
+      </c>
+      <c r="C5">
+        <f>COUNTIFS(SEMUA!$F$1:$F$255,rekap!$C$2,SEMUA!$E$1:$E$255,rekap!B5)</f>
+        <v>52</v>
+      </c>
+      <c r="D5">
+        <f>COUNTIFS(SEMUA!$F$1:$F$255,rekap!$D$2,SEMUA!$E$1:$E$255,rekap!B5)</f>
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>54</v>
+      </c>
+      <c r="G5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="15">
+        <v>56</v>
+      </c>
+      <c r="C6">
+        <f>COUNTIFS(SEMUA!$F$1:$F$255,rekap!$C$2,SEMUA!$E$1:$E$255,rekap!B6)</f>
+        <v>72</v>
+      </c>
+      <c r="D6">
+        <f>COUNTIFS(SEMUA!$F$1:$F$255,rekap!$D$2,SEMUA!$E$1:$E$255,rekap!B6)</f>
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>74</v>
+      </c>
+      <c r="G6">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="14">
+        <v>57</v>
+      </c>
+      <c r="C7">
+        <f>COUNTIFS(SEMUA!$F$1:$F$255,rekap!$C$2,SEMUA!$E$1:$E$255,rekap!B7)</f>
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <f>COUNTIFS(SEMUA!$F$1:$F$255,rekap!$D$2,SEMUA!$E$1:$E$255,rekap!B7)</f>
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>32</v>
+      </c>
+      <c r="G7">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="15">
+        <v>58</v>
+      </c>
+      <c r="C8">
+        <f>COUNTIFS(SEMUA!$F$1:$F$255,rekap!$C$2,SEMUA!$E$1:$E$255,rekap!B8)</f>
+        <v>27</v>
+      </c>
+      <c r="D8">
+        <f>COUNTIFS(SEMUA!$F$1:$F$255,rekap!$D$2,SEMUA!$E$1:$E$255,rekap!B8)</f>
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>27</v>
+      </c>
+      <c r="G8">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="14">
+        <v>59</v>
+      </c>
+      <c r="C9">
+        <f>COUNTIFS(SEMUA!$F$1:$F$255,rekap!$C$2,SEMUA!$E$1:$E$255,rekap!B9)</f>
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <f>COUNTIFS(SEMUA!$F$1:$F$255,rekap!$D$2,SEMUA!$E$1:$E$255,rekap!B9)</f>
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="15">
+        <v>60</v>
+      </c>
+      <c r="C10">
+        <f>COUNTIFS(SEMUA!$F$1:$F$255,rekap!$C$2,SEMUA!$E$1:$E$255,rekap!B10)</f>
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <f>COUNTIFS(SEMUA!$F$1:$F$255,rekap!$D$2,SEMUA!$E$1:$E$255,rekap!B10)</f>
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="14"/>
+      <c r="C11">
+        <f>SUM(C3:C10)</f>
+        <v>220</v>
+      </c>
+      <c r="D11">
+        <f>SUM(D3:D10)</f>
+        <v>27</v>
+      </c>
+      <c r="E11">
+        <f>SUM(E3:E10)</f>
+        <v>227</v>
+      </c>
+      <c r="G11">
+        <f>SUM(G3:G10)</f>
+        <v>254</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:B256">
+    <sortCondition ref="B3:B256"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56540605-357D-4090-96BB-A07ECC59CF0C}">
   <dimension ref="A3:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="C38" sqref="C38:C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
cetak taruna ke 2
</commit_message>
<xml_diff>
--- a/27. TARUNA 2021-2 E(K_1) N(K_2) T(K_3)/UKURAN.xlsx
+++ b/27. TARUNA 2021-2 E(K_1) N(K_2) T(K_3)/UKURAN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mapan\progress\27. TARUNA 2021-2 E(K_1) N(K_2) T(K_3)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3F17F8-C43B-4211-998D-DDEE53B819E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6791B5E-21D9-4512-85FB-E43D07E916AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="23925" xr2:uid="{8D0EA34A-D090-461B-B73E-10F00D55D97B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D0EA34A-D090-461B-B73E-10F00D55D97B}"/>
   </bookViews>
   <sheets>
     <sheet name="SEMUA" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1328" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1332" uniqueCount="571">
   <si>
     <t>ARUM PAMBUDININGTYAS</t>
   </si>
@@ -1741,6 +1741,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>28 agust</t>
   </si>
 </sst>
 </file>
@@ -2386,12 +2389,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0593BD49-364B-49CF-AB09-840279B88535}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:Z536"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="55" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A231" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W256" sqref="W256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2490,7 +2492,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="23.25" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="23.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>208</v>
       </c>
@@ -2564,7 +2566,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>209</v>
       </c>
@@ -2638,7 +2640,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>210</v>
       </c>
@@ -2712,7 +2714,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>211</v>
       </c>
@@ -2786,7 +2788,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="23.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>212</v>
       </c>
@@ -2860,7 +2862,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>213</v>
       </c>
@@ -2934,7 +2936,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>214</v>
       </c>
@@ -3008,7 +3010,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>215</v>
       </c>
@@ -3082,7 +3084,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>216</v>
       </c>
@@ -3156,7 +3158,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>217</v>
       </c>
@@ -3230,7 +3232,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>218</v>
       </c>
@@ -3452,7 +3454,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>221</v>
       </c>
@@ -3526,7 +3528,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>222</v>
       </c>
@@ -3600,7 +3602,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="17" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>223</v>
       </c>
@@ -3674,7 +3676,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>224</v>
       </c>
@@ -3748,7 +3750,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>225</v>
       </c>
@@ -3896,7 +3898,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>227</v>
       </c>
@@ -3970,7 +3972,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>228</v>
       </c>
@@ -4044,7 +4046,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>229</v>
       </c>
@@ -4118,7 +4120,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="24" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>230</v>
       </c>
@@ -4192,7 +4194,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>231</v>
       </c>
@@ -4266,7 +4268,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="26" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>232</v>
       </c>
@@ -4340,7 +4342,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="27" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>233</v>
       </c>
@@ -4414,7 +4416,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>234</v>
       </c>
@@ -4636,7 +4638,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="31" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>237</v>
       </c>
@@ -4784,7 +4786,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="33" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>239</v>
       </c>
@@ -4858,7 +4860,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="34" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>240</v>
       </c>
@@ -4932,7 +4934,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="35" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>241</v>
       </c>
@@ -5006,7 +5008,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="36" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>242</v>
       </c>
@@ -5228,7 +5230,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="39" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>245</v>
       </c>
@@ -5302,7 +5304,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="40" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>246</v>
       </c>
@@ -5376,7 +5378,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="41" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>247</v>
       </c>
@@ -5450,7 +5452,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="42" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>248</v>
       </c>
@@ -5524,7 +5526,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="43" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>249</v>
       </c>
@@ -5598,7 +5600,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="44" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>250</v>
       </c>
@@ -5672,7 +5674,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="45" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>251</v>
       </c>
@@ -5746,7 +5748,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="46" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>252</v>
       </c>
@@ -5820,7 +5822,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="47" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>253</v>
       </c>
@@ -5894,7 +5896,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="48" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>254</v>
       </c>
@@ -5968,7 +5970,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="49" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>255</v>
       </c>
@@ -6042,7 +6044,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="50" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>256</v>
       </c>
@@ -6116,7 +6118,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="51" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>257</v>
       </c>
@@ -6190,7 +6192,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="52" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>258</v>
       </c>
@@ -6264,7 +6266,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="53" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>259</v>
       </c>
@@ -6338,7 +6340,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="54" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>260</v>
       </c>
@@ -6412,7 +6414,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="55" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
         <v>261</v>
       </c>
@@ -6486,7 +6488,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="56" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>262</v>
       </c>
@@ -6560,7 +6562,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="57" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>263</v>
       </c>
@@ -6782,7 +6784,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="60" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>266</v>
       </c>
@@ -6856,7 +6858,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="61" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
         <v>267</v>
       </c>
@@ -6930,7 +6932,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="62" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>268</v>
       </c>
@@ -6997,8 +6999,14 @@
       <c r="V62" s="4">
         <v>91</v>
       </c>
-    </row>
-    <row r="63" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W62" s="4">
+        <v>2</v>
+      </c>
+      <c r="X62" s="4" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
         <v>269</v>
       </c>
@@ -7065,8 +7073,14 @@
       <c r="V63" s="4">
         <v>95</v>
       </c>
-    </row>
-    <row r="64" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W63" s="4">
+        <v>2</v>
+      </c>
+      <c r="X63" s="4" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>270</v>
       </c>
@@ -7140,7 +7154,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="65" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
         <v>271</v>
       </c>
@@ -7214,7 +7228,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="66" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>272</v>
       </c>
@@ -7288,7 +7302,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="67" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
         <v>273</v>
       </c>
@@ -7436,7 +7450,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="69" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
         <v>275</v>
       </c>
@@ -7584,7 +7598,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="71" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
         <v>277</v>
       </c>
@@ -7658,7 +7672,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="72" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>278</v>
       </c>
@@ -7732,7 +7746,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="73" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
         <v>279</v>
       </c>
@@ -7806,7 +7820,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="74" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>280</v>
       </c>
@@ -7880,7 +7894,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="75" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
         <v>281</v>
       </c>
@@ -7954,7 +7968,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="76" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>282</v>
       </c>
@@ -8028,7 +8042,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="77" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
         <v>283</v>
       </c>
@@ -8102,7 +8116,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="78" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>284</v>
       </c>
@@ -8176,7 +8190,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="79" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
         <v>285</v>
       </c>
@@ -8250,7 +8264,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="80" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>286</v>
       </c>
@@ -8324,7 +8338,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="81" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
         <v>287</v>
       </c>
@@ -8398,7 +8412,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="82" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>288</v>
       </c>
@@ -8472,7 +8486,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="83" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
         <v>289</v>
       </c>
@@ -8546,7 +8560,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="84" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>290</v>
       </c>
@@ -8620,7 +8634,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="85" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
         <v>291</v>
       </c>
@@ -8694,7 +8708,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="86" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>292</v>
       </c>
@@ -8842,7 +8856,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="88" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>294</v>
       </c>
@@ -8916,7 +8930,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="89" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
         <v>295</v>
       </c>
@@ -8990,7 +9004,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="90" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>296</v>
       </c>
@@ -9064,7 +9078,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="91" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
         <v>297</v>
       </c>
@@ -9138,7 +9152,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="92" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>298</v>
       </c>
@@ -9205,8 +9219,14 @@
       <c r="V92" s="4">
         <v>94</v>
       </c>
-    </row>
-    <row r="93" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W92" s="4">
+        <v>2</v>
+      </c>
+      <c r="X92" s="4" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="93" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="11" t="s">
         <v>299</v>
       </c>
@@ -9354,7 +9374,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="95" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
         <v>301</v>
       </c>
@@ -9428,7 +9448,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="96" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>302</v>
       </c>
@@ -9650,7 +9670,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="99" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
         <v>305</v>
       </c>
@@ -9724,7 +9744,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="100" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>306</v>
       </c>
@@ -9798,7 +9818,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="101" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="11" t="s">
         <v>307</v>
       </c>
@@ -9872,7 +9892,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="102" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>308</v>
       </c>
@@ -9946,7 +9966,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="103" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
         <v>309</v>
       </c>
@@ -10020,7 +10040,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="104" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>310</v>
       </c>
@@ -10168,7 +10188,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="106" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>312</v>
       </c>
@@ -10242,7 +10262,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="107" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
         <v>313</v>
       </c>
@@ -10316,7 +10336,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="108" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>314</v>
       </c>
@@ -10390,7 +10410,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="109" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
         <v>315</v>
       </c>
@@ -10464,7 +10484,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="110" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>316</v>
       </c>
@@ -10538,7 +10558,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="111" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
         <v>317</v>
       </c>
@@ -10612,7 +10632,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="112" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>318</v>
       </c>
@@ -10760,7 +10780,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="114" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>320</v>
       </c>
@@ -10834,7 +10854,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="115" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="11" t="s">
         <v>321</v>
       </c>
@@ -10908,7 +10928,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="116" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>322</v>
       </c>
@@ -10982,7 +11002,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="117" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="11" t="s">
         <v>323</v>
       </c>
@@ -11056,7 +11076,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="118" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="26" t="s">
         <v>324</v>
       </c>
@@ -11090,7 +11110,7 @@
       <c r="W118" s="41"/>
       <c r="X118" s="41"/>
     </row>
-    <row r="119" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="11" t="s">
         <v>325</v>
       </c>
@@ -11164,7 +11184,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="120" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>326</v>
       </c>
@@ -11238,7 +11258,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="121" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="11" t="s">
         <v>327</v>
       </c>
@@ -11460,7 +11480,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="124" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>330</v>
       </c>
@@ -11534,7 +11554,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="125" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="11" t="s">
         <v>331</v>
       </c>
@@ -11608,7 +11628,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="126" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>332</v>
       </c>
@@ -11682,7 +11702,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="127" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="11" t="s">
         <v>333</v>
       </c>
@@ -11821,7 +11841,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="129" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="11" t="s">
         <v>335</v>
       </c>
@@ -11895,7 +11915,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="130" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>336</v>
       </c>
@@ -12034,7 +12054,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="132" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>338</v>
       </c>
@@ -12108,7 +12128,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="133" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="32" t="s">
         <v>339</v>
       </c>
@@ -12142,7 +12162,7 @@
       <c r="W133" s="41"/>
       <c r="X133" s="41"/>
     </row>
-    <row r="134" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>340</v>
       </c>
@@ -12216,7 +12236,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="135" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="11" t="s">
         <v>341</v>
       </c>
@@ -12290,7 +12310,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="136" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>342</v>
       </c>
@@ -12364,7 +12384,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="137" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="11" t="s">
         <v>343</v>
       </c>
@@ -12438,7 +12458,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="138" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>344</v>
       </c>
@@ -12660,7 +12680,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="141" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="11" t="s">
         <v>347</v>
       </c>
@@ -12808,7 +12828,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="143" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="11" t="s">
         <v>349</v>
       </c>
@@ -12882,7 +12902,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="144" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>350</v>
       </c>
@@ -12956,7 +12976,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="145" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="11" t="s">
         <v>351</v>
       </c>
@@ -13030,7 +13050,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="146" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>352</v>
       </c>
@@ -13104,7 +13124,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="147" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="11" t="s">
         <v>353</v>
       </c>
@@ -13178,7 +13198,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="148" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>354</v>
       </c>
@@ -13252,7 +13272,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="149" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="11" t="s">
         <v>355</v>
       </c>
@@ -13326,7 +13346,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="150" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>356</v>
       </c>
@@ -13400,7 +13420,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="151" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="11" t="s">
         <v>357</v>
       </c>
@@ -13474,7 +13494,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="152" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="26" t="s">
         <v>358</v>
       </c>
@@ -13508,7 +13528,7 @@
       <c r="W152" s="41"/>
       <c r="X152" s="41"/>
     </row>
-    <row r="153" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>568</v>
       </c>
@@ -13575,8 +13595,14 @@
       <c r="V153" s="4">
         <v>92</v>
       </c>
-    </row>
-    <row r="154" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W153" s="4">
+        <v>2</v>
+      </c>
+      <c r="X153" s="4" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="154" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="11" t="s">
         <v>359</v>
       </c>
@@ -13650,7 +13676,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="155" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="9" t="s">
         <v>360</v>
       </c>
@@ -13724,7 +13750,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="156" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="11" t="s">
         <v>361</v>
       </c>
@@ -13798,7 +13824,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="157" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="9" t="s">
         <v>362</v>
       </c>
@@ -13872,7 +13898,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="158" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="11" t="s">
         <v>363</v>
       </c>
@@ -13946,7 +13972,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="159" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="9" t="s">
         <v>364</v>
       </c>
@@ -14020,7 +14046,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="160" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="11" t="s">
         <v>365</v>
       </c>
@@ -14094,7 +14120,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="161" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="9" t="s">
         <v>366</v>
       </c>
@@ -14168,7 +14194,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="162" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="11" t="s">
         <v>367</v>
       </c>
@@ -14242,7 +14268,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="163" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="9" t="s">
         <v>368</v>
       </c>
@@ -14316,7 +14342,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="164" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="11" t="s">
         <v>369</v>
       </c>
@@ -14390,7 +14416,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="165" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="9" t="s">
         <v>370</v>
       </c>
@@ -14464,7 +14490,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="166" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="11" t="s">
         <v>371</v>
       </c>
@@ -14538,7 +14564,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="167" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="9" t="s">
         <v>372</v>
       </c>
@@ -14612,7 +14638,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="168" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="11" t="s">
         <v>373</v>
       </c>
@@ -14686,7 +14712,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="169" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="9" t="s">
         <v>374</v>
       </c>
@@ -14760,7 +14786,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="170" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="11" t="s">
         <v>375</v>
       </c>
@@ -14834,7 +14860,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="171" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="9" t="s">
         <v>376</v>
       </c>
@@ -14908,7 +14934,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="172" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="11" t="s">
         <v>377</v>
       </c>
@@ -14982,7 +15008,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="173" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="9" t="s">
         <v>378</v>
       </c>
@@ -15056,7 +15082,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="174" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="11" t="s">
         <v>379</v>
       </c>
@@ -15130,7 +15156,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="175" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="9" t="s">
         <v>380</v>
       </c>
@@ -15204,7 +15230,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="176" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="11" t="s">
         <v>381</v>
       </c>
@@ -15352,7 +15378,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="178" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="11" t="s">
         <v>383</v>
       </c>
@@ -15426,7 +15452,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="179" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="9" t="s">
         <v>384</v>
       </c>
@@ -15500,7 +15526,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="180" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="11" t="s">
         <v>385</v>
       </c>
@@ -15574,7 +15600,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="181" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="9" t="s">
         <v>386</v>
       </c>
@@ -15648,7 +15674,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="182" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="11" t="s">
         <v>387</v>
       </c>
@@ -15722,7 +15748,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="183" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="9" t="s">
         <v>388</v>
       </c>
@@ -15796,7 +15822,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="184" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="11" t="s">
         <v>389</v>
       </c>
@@ -15870,7 +15896,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="185" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="9" t="s">
         <v>390</v>
       </c>
@@ -15944,7 +15970,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="186" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="11" t="s">
         <v>391</v>
       </c>
@@ -16018,7 +16044,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="187" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="9" t="s">
         <v>392</v>
       </c>
@@ -16092,7 +16118,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="188" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="11" t="s">
         <v>393</v>
       </c>
@@ -16166,7 +16192,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="189" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="9" t="s">
         <v>394</v>
       </c>
@@ -16240,7 +16266,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="190" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="11" t="s">
         <v>395</v>
       </c>
@@ -16314,7 +16340,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="191" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="9" t="s">
         <v>396</v>
       </c>
@@ -16388,7 +16414,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="192" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="11" t="s">
         <v>397</v>
       </c>
@@ -16462,7 +16488,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="193" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="9" t="s">
         <v>398</v>
       </c>
@@ -16536,7 +16562,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="194" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="11" t="s">
         <v>399</v>
       </c>
@@ -16610,7 +16636,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="195" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="9" t="s">
         <v>400</v>
       </c>
@@ -16684,7 +16710,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="196" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="11" t="s">
         <v>401</v>
       </c>
@@ -16758,7 +16784,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="197" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="9" t="s">
         <v>402</v>
       </c>
@@ -16832,7 +16858,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="198" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="11" t="s">
         <v>403</v>
       </c>
@@ -16906,7 +16932,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="199" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="9" t="s">
         <v>404</v>
       </c>
@@ -16980,7 +17006,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="200" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="11" t="s">
         <v>405</v>
       </c>
@@ -17054,7 +17080,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="201" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="9" t="s">
         <v>406</v>
       </c>
@@ -17128,7 +17154,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="202" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="11" t="s">
         <v>407</v>
       </c>
@@ -17202,7 +17228,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="203" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="9" t="s">
         <v>408</v>
       </c>
@@ -17276,7 +17302,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="204" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="11" t="s">
         <v>409</v>
       </c>
@@ -17350,7 +17376,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="205" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="9" t="s">
         <v>410</v>
       </c>
@@ -17424,7 +17450,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="206" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="11" t="s">
         <v>411</v>
       </c>
@@ -17498,7 +17524,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="207" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="9" t="s">
         <v>412</v>
       </c>
@@ -17572,7 +17598,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="208" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="11" t="s">
         <v>413</v>
       </c>
@@ -17646,7 +17672,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="9" t="s">
         <v>414</v>
       </c>
@@ -17720,7 +17746,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="210" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="11" t="s">
         <v>415</v>
       </c>
@@ -17794,7 +17820,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="211" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="9" t="s">
         <v>416</v>
       </c>
@@ -17868,7 +17894,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="212" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="11" t="s">
         <v>417</v>
       </c>
@@ -17942,7 +17968,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="213" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="9" t="s">
         <v>418</v>
       </c>
@@ -18016,7 +18042,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="214" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="11" t="s">
         <v>419</v>
       </c>
@@ -18090,7 +18116,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="215" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="9" t="s">
         <v>420</v>
       </c>
@@ -18164,7 +18190,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="216" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="11" t="s">
         <v>421</v>
       </c>
@@ -18238,7 +18264,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="217" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="9" t="s">
         <v>422</v>
       </c>
@@ -18312,7 +18338,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="218" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="11" t="s">
         <v>423</v>
       </c>
@@ -18386,7 +18412,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="219" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="9" t="s">
         <v>424</v>
       </c>
@@ -18460,7 +18486,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="220" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="11" t="s">
         <v>425</v>
       </c>
@@ -18534,7 +18560,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="221" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="9" t="s">
         <v>426</v>
       </c>
@@ -18608,7 +18634,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="222" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="11" t="s">
         <v>427</v>
       </c>
@@ -18682,7 +18708,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="223" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="9" t="s">
         <v>428</v>
       </c>
@@ -18756,7 +18782,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="224" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="11" t="s">
         <v>429</v>
       </c>
@@ -18830,7 +18856,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="225" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="9" t="s">
         <v>430</v>
       </c>
@@ -18904,7 +18930,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="226" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="11" t="s">
         <v>431</v>
       </c>
@@ -18978,7 +19004,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="227" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="9" t="s">
         <v>432</v>
       </c>
@@ -19052,7 +19078,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="228" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="11" t="s">
         <v>433</v>
       </c>
@@ -19126,7 +19152,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="229" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="9" t="s">
         <v>434</v>
       </c>
@@ -19200,7 +19226,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="230" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="11" t="s">
         <v>435</v>
       </c>
@@ -19274,7 +19300,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="231" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="9" t="s">
         <v>436</v>
       </c>
@@ -19348,7 +19374,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="232" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="11" t="s">
         <v>437</v>
       </c>
@@ -19422,7 +19448,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="233" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="9" t="s">
         <v>438</v>
       </c>
@@ -19496,7 +19522,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="234" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="11" t="s">
         <v>439</v>
       </c>
@@ -19570,7 +19596,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="235" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="9" t="s">
         <v>440</v>
       </c>
@@ -19644,7 +19670,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="236" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="11" t="s">
         <v>441</v>
       </c>
@@ -19670,7 +19696,7 @@
       <c r="O236" s="20"/>
       <c r="P236" s="39"/>
     </row>
-    <row r="237" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="9" t="s">
         <v>442</v>
       </c>
@@ -19744,7 +19770,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="238" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="11" t="s">
         <v>443</v>
       </c>
@@ -19818,7 +19844,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="239" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="9" t="s">
         <v>444</v>
       </c>
@@ -19892,7 +19918,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="240" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="11" t="s">
         <v>445</v>
       </c>
@@ -19966,7 +19992,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="241" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="9" t="s">
         <v>446</v>
       </c>
@@ -20040,7 +20066,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="242" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="11" t="s">
         <v>447</v>
       </c>
@@ -20114,7 +20140,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="243" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="9" t="s">
         <v>448</v>
       </c>
@@ -20188,7 +20214,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="244" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="11" t="s">
         <v>449</v>
       </c>
@@ -20262,7 +20288,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="245" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="9" t="s">
         <v>450</v>
       </c>
@@ -20336,7 +20362,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="246" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="11" t="s">
         <v>451</v>
       </c>
@@ -20410,7 +20436,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="247" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="9" t="s">
         <v>452</v>
       </c>
@@ -20484,7 +20510,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="248" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="11" t="s">
         <v>453</v>
       </c>
@@ -20558,7 +20584,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="249" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="9" t="s">
         <v>454</v>
       </c>
@@ -20632,7 +20658,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="250" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="11" t="s">
         <v>455</v>
       </c>
@@ -20706,7 +20732,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="251" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="9" t="s">
         <v>456</v>
       </c>
@@ -20780,7 +20806,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="252" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="11" t="s">
         <v>457</v>
       </c>
@@ -20854,7 +20880,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="253" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="9" t="s">
         <v>458</v>
       </c>
@@ -20928,7 +20954,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="254" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="11" t="s">
         <v>459</v>
       </c>
@@ -21002,7 +21028,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="255" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="9" t="s">
         <v>460</v>
       </c>
@@ -21076,7 +21102,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="256" spans="1:24" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="11" t="s">
         <v>461</v>
       </c>
@@ -25939,13 +25965,6 @@
       <c r="L536" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z256" xr:uid="{0593BD49-364B-49CF-AB09-840279B88535}">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="WANITA"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.43307086614173229" right="0.11811023622047245" top="0.51181102362204722" bottom="0.19685039370078741" header="0.19685039370078741" footer="0.11811023622047245"/>

</xml_diff>

<commit_message>
cetak kaos dan sepatu dp
</commit_message>
<xml_diff>
--- a/27. TARUNA 2021-2 E(K_1) N(K_2) T(K_3)/UKURAN.xlsx
+++ b/27. TARUNA 2021-2 E(K_1) N(K_2) T(K_3)/UKURAN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mapan\progress\27. TARUNA 2021-2 E(K_1) N(K_2) T(K_3)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549CA8A2-7BF2-4921-A56F-D1EA83BB534E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7F3F19-15D5-442E-B15E-ACD010F8C482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D0EA34A-D090-461B-B73E-10F00D55D97B}"/>
   </bookViews>
@@ -1942,7 +1942,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2080,21 +2080,18 @@
     <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{2F7A6239-2CAD-4641-BDE2-E1026B3F7379}"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC00000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2404,12 +2401,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0593BD49-364B-49CF-AB09-840279B88535}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:Z536"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y152" sqref="Y152"/>
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2510,7 +2506,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="23.25" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="23.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>208</v>
       </c>
@@ -2586,8 +2582,11 @@
       <c r="Y2" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z2" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>209</v>
       </c>
@@ -2663,8 +2662,11 @@
       <c r="Y3" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z3" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>210</v>
       </c>
@@ -2740,8 +2742,11 @@
       <c r="Y4" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z4" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>211</v>
       </c>
@@ -2817,8 +2822,11 @@
       <c r="Y5" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z5" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>212</v>
       </c>
@@ -2894,8 +2902,11 @@
       <c r="Y6" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z6" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>213</v>
       </c>
@@ -2971,8 +2982,11 @@
       <c r="Y7" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z7" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>214</v>
       </c>
@@ -3048,8 +3062,11 @@
       <c r="Y8" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z8" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>215</v>
       </c>
@@ -3125,8 +3142,11 @@
       <c r="Y9" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z9" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>216</v>
       </c>
@@ -3202,8 +3222,11 @@
       <c r="Y10" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z10" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>217</v>
       </c>
@@ -3279,8 +3302,11 @@
       <c r="Y11" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z11" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>218</v>
       </c>
@@ -3356,8 +3382,11 @@
       <c r="Y12" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z12" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>219</v>
       </c>
@@ -3433,8 +3462,11 @@
       <c r="Y13" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z13" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>220</v>
       </c>
@@ -3510,8 +3542,11 @@
       <c r="Y14" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z14" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>221</v>
       </c>
@@ -3587,8 +3622,11 @@
       <c r="Y15" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z15" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>222</v>
       </c>
@@ -3664,8 +3702,11 @@
       <c r="Y16" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z16" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>223</v>
       </c>
@@ -3741,8 +3782,11 @@
       <c r="Y17" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z17" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>224</v>
       </c>
@@ -3818,8 +3862,11 @@
       <c r="Y18" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z18" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>225</v>
       </c>
@@ -3895,8 +3942,11 @@
       <c r="Y19" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z19" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>226</v>
       </c>
@@ -3972,8 +4022,11 @@
       <c r="Y20" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z20" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>227</v>
       </c>
@@ -4049,8 +4102,11 @@
       <c r="Y21" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="22" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z21" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>228</v>
       </c>
@@ -4126,8 +4182,11 @@
       <c r="Y22" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="23" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z22" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>229</v>
       </c>
@@ -4203,8 +4262,11 @@
       <c r="Y23" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z23" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>230</v>
       </c>
@@ -4280,8 +4342,11 @@
       <c r="Y24" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="25" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z24" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>231</v>
       </c>
@@ -4357,8 +4422,11 @@
       <c r="Y25" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="26" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z25" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>232</v>
       </c>
@@ -4434,8 +4502,11 @@
       <c r="Y26" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z26" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>233</v>
       </c>
@@ -4511,8 +4582,11 @@
       <c r="Y27" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="28" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z27" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>234</v>
       </c>
@@ -4588,8 +4662,11 @@
       <c r="Y28" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z28" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>235</v>
       </c>
@@ -4665,8 +4742,11 @@
       <c r="Y29" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="30" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z29" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>236</v>
       </c>
@@ -4742,8 +4822,11 @@
       <c r="Y30" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="31" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z30" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>237</v>
       </c>
@@ -4819,8 +4902,11 @@
       <c r="Y31" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="32" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z31" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>238</v>
       </c>
@@ -4896,8 +4982,11 @@
       <c r="Y32" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="33" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z32" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>239</v>
       </c>
@@ -4973,8 +5062,11 @@
       <c r="Y33" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="34" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z33" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>240</v>
       </c>
@@ -5050,8 +5142,11 @@
       <c r="Y34" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="35" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z34" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>241</v>
       </c>
@@ -5127,8 +5222,11 @@
       <c r="Y35" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="36" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z35" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>242</v>
       </c>
@@ -5204,8 +5302,11 @@
       <c r="Y36" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="37" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z36" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>243</v>
       </c>
@@ -5281,8 +5382,11 @@
       <c r="Y37" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="38" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z37" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>244</v>
       </c>
@@ -5358,8 +5462,11 @@
       <c r="Y38" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="39" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z38" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>245</v>
       </c>
@@ -5435,8 +5542,11 @@
       <c r="Y39" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="40" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z39" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>246</v>
       </c>
@@ -5512,8 +5622,11 @@
       <c r="Y40" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="41" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z40" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>247</v>
       </c>
@@ -5589,8 +5702,11 @@
       <c r="Y41" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="42" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z41" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>248</v>
       </c>
@@ -5666,8 +5782,11 @@
       <c r="Y42" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="43" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z42" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>249</v>
       </c>
@@ -5743,8 +5862,11 @@
       <c r="Y43" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="44" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z43" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>250</v>
       </c>
@@ -5820,8 +5942,11 @@
       <c r="Y44" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="45" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z44" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>251</v>
       </c>
@@ -5897,8 +6022,11 @@
       <c r="Y45" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="46" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z45" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>252</v>
       </c>
@@ -5974,8 +6102,11 @@
       <c r="Y46" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="47" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z46" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>253</v>
       </c>
@@ -6051,8 +6182,11 @@
       <c r="Y47" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="48" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z47" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>254</v>
       </c>
@@ -6128,8 +6262,11 @@
       <c r="Y48" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="49" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z48" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>255</v>
       </c>
@@ -6205,8 +6342,11 @@
       <c r="Y49" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="50" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z49" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>256</v>
       </c>
@@ -6282,8 +6422,11 @@
       <c r="Y50" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="51" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z50" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>257</v>
       </c>
@@ -6359,8 +6502,11 @@
       <c r="Y51" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="52" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z51" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>258</v>
       </c>
@@ -6436,8 +6582,11 @@
       <c r="Y52" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="53" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z52" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>259</v>
       </c>
@@ -6513,8 +6662,11 @@
       <c r="Y53" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="54" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z53" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>260</v>
       </c>
@@ -6590,8 +6742,11 @@
       <c r="Y54" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="55" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z54" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
         <v>261</v>
       </c>
@@ -6667,8 +6822,11 @@
       <c r="Y55" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="56" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z55" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>262</v>
       </c>
@@ -6744,8 +6902,11 @@
       <c r="Y56" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="57" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z56" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>263</v>
       </c>
@@ -6821,8 +6982,11 @@
       <c r="Y57" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="58" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z57" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>264</v>
       </c>
@@ -6898,8 +7062,11 @@
       <c r="Y58" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="59" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z58" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="59" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
         <v>265</v>
       </c>
@@ -6975,8 +7142,11 @@
       <c r="Y59" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="60" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z59" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="60" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>266</v>
       </c>
@@ -7052,8 +7222,11 @@
       <c r="Y60" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="61" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z60" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="61" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
         <v>267</v>
       </c>
@@ -7129,8 +7302,11 @@
       <c r="Y61" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="62" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z61" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="62" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>268</v>
       </c>
@@ -7206,8 +7382,11 @@
       <c r="Y62" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="63" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z62" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="63" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
         <v>269</v>
       </c>
@@ -7283,8 +7462,11 @@
       <c r="Y63" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="64" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z63" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="64" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>270</v>
       </c>
@@ -7360,8 +7542,11 @@
       <c r="Y64" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="65" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z64" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="65" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
         <v>271</v>
       </c>
@@ -7437,8 +7622,11 @@
       <c r="Y65" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="66" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z65" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="66" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>272</v>
       </c>
@@ -7514,8 +7702,11 @@
       <c r="Y66" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="67" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z66" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
         <v>273</v>
       </c>
@@ -7591,8 +7782,11 @@
       <c r="Y67" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="68" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z67" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="68" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>274</v>
       </c>
@@ -7668,8 +7862,11 @@
       <c r="Y68" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="69" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z68" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="69" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
         <v>275</v>
       </c>
@@ -7745,8 +7942,11 @@
       <c r="Y69" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="70" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z69" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="70" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>276</v>
       </c>
@@ -7822,8 +8022,11 @@
       <c r="Y70" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="71" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z70" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="71" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
         <v>277</v>
       </c>
@@ -7899,8 +8102,11 @@
       <c r="Y71" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="72" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z71" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="72" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>278</v>
       </c>
@@ -7976,8 +8182,11 @@
       <c r="Y72" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="73" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z72" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="73" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
         <v>279</v>
       </c>
@@ -8053,8 +8262,11 @@
       <c r="Y73" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="74" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z73" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="74" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>280</v>
       </c>
@@ -8130,8 +8342,11 @@
       <c r="Y74" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="75" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z74" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="75" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
         <v>281</v>
       </c>
@@ -8207,8 +8422,11 @@
       <c r="Y75" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="76" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z75" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="76" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>282</v>
       </c>
@@ -8284,8 +8502,11 @@
       <c r="Y76" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="77" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z76" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="77" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
         <v>283</v>
       </c>
@@ -8361,8 +8582,11 @@
       <c r="Y77" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="78" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z77" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="78" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>284</v>
       </c>
@@ -8438,8 +8662,11 @@
       <c r="Y78" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="79" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z78" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="79" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
         <v>285</v>
       </c>
@@ -8515,8 +8742,11 @@
       <c r="Y79" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="80" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z79" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="80" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>286</v>
       </c>
@@ -8592,8 +8822,11 @@
       <c r="Y80" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="81" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z80" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="81" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
         <v>287</v>
       </c>
@@ -8669,8 +8902,11 @@
       <c r="Y81" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="82" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z81" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="82" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>288</v>
       </c>
@@ -8746,8 +8982,11 @@
       <c r="Y82" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="83" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z82" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="83" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
         <v>289</v>
       </c>
@@ -8823,8 +9062,11 @@
       <c r="Y83" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="84" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z83" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="84" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>290</v>
       </c>
@@ -8900,8 +9142,11 @@
       <c r="Y84" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="85" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z84" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="85" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
         <v>291</v>
       </c>
@@ -8977,8 +9222,11 @@
       <c r="Y85" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="86" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z85" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="86" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>292</v>
       </c>
@@ -9054,8 +9302,11 @@
       <c r="Y86" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="87" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z86" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="87" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
         <v>293</v>
       </c>
@@ -9131,8 +9382,11 @@
       <c r="Y87" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="88" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z87" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="88" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>294</v>
       </c>
@@ -9208,8 +9462,11 @@
       <c r="Y88" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="89" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z88" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="89" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
         <v>295</v>
       </c>
@@ -9285,8 +9542,11 @@
       <c r="Y89" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="90" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z89" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="90" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>296</v>
       </c>
@@ -9362,8 +9622,11 @@
       <c r="Y90" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="91" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z90" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="91" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="11" t="s">
         <v>297</v>
       </c>
@@ -9439,8 +9702,11 @@
       <c r="Y91" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="92" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z91" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="92" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>298</v>
       </c>
@@ -9516,8 +9782,11 @@
       <c r="Y92" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="93" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z92" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="93" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="11" t="s">
         <v>299</v>
       </c>
@@ -9593,8 +9862,11 @@
       <c r="Y93" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="94" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z93" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="94" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>300</v>
       </c>
@@ -9670,8 +9942,11 @@
       <c r="Y94" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="95" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z94" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="95" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
         <v>301</v>
       </c>
@@ -9747,8 +10022,11 @@
       <c r="Y95" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="96" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z95" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="96" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>302</v>
       </c>
@@ -9824,8 +10102,11 @@
       <c r="Y96" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="97" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z96" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="97" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
         <v>303</v>
       </c>
@@ -9901,8 +10182,11 @@
       <c r="Y97" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="98" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z97" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="98" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>304</v>
       </c>
@@ -9978,8 +10262,11 @@
       <c r="Y98" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="99" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z98" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="99" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="11" t="s">
         <v>305</v>
       </c>
@@ -10055,8 +10342,11 @@
       <c r="Y99" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="100" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z99" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="100" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>306</v>
       </c>
@@ -10132,8 +10422,11 @@
       <c r="Y100" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="101" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z100" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="101" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="11" t="s">
         <v>307</v>
       </c>
@@ -10209,8 +10502,11 @@
       <c r="Y101" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="102" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z101" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="102" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>308</v>
       </c>
@@ -10286,8 +10582,11 @@
       <c r="Y102" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="103" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z102" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="103" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="11" t="s">
         <v>309</v>
       </c>
@@ -10363,8 +10662,11 @@
       <c r="Y103" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="104" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z103" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="104" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>310</v>
       </c>
@@ -10440,8 +10742,11 @@
       <c r="Y104" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="105" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z104" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="105" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="11" t="s">
         <v>311</v>
       </c>
@@ -10517,8 +10822,11 @@
       <c r="Y105" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="106" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z105" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="106" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>312</v>
       </c>
@@ -10594,8 +10902,11 @@
       <c r="Y106" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="107" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z106" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="107" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="11" t="s">
         <v>313</v>
       </c>
@@ -10671,8 +10982,11 @@
       <c r="Y107" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="108" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z107" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="108" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>314</v>
       </c>
@@ -10748,8 +11062,11 @@
       <c r="Y108" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="109" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z108" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="109" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="11" t="s">
         <v>315</v>
       </c>
@@ -10825,8 +11142,11 @@
       <c r="Y109" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="110" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z109" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="110" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>316</v>
       </c>
@@ -10902,8 +11222,11 @@
       <c r="Y110" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="111" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z110" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="111" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="11" t="s">
         <v>317</v>
       </c>
@@ -10979,8 +11302,11 @@
       <c r="Y111" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="112" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z111" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="112" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>318</v>
       </c>
@@ -11056,8 +11382,11 @@
       <c r="Y112" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="113" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z112" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="113" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="11" t="s">
         <v>319</v>
       </c>
@@ -11133,8 +11462,11 @@
       <c r="Y113" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="114" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z113" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="114" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>320</v>
       </c>
@@ -11210,8 +11542,11 @@
       <c r="Y114" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="115" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z114" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="115" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="11" t="s">
         <v>321</v>
       </c>
@@ -11287,8 +11622,11 @@
       <c r="Y115" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="116" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z115" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="116" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>322</v>
       </c>
@@ -11364,8 +11702,11 @@
       <c r="Y116" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="117" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z116" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="117" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="11" t="s">
         <v>323</v>
       </c>
@@ -11441,8 +11782,11 @@
       <c r="Y117" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="118" spans="1:25" ht="23.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="Z117" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="118" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="26" t="s">
         <v>324</v>
       </c>
@@ -11476,8 +11820,9 @@
       <c r="W118" s="41"/>
       <c r="X118" s="41"/>
       <c r="Y118" s="46"/>
-    </row>
-    <row r="119" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z118" s="46"/>
+    </row>
+    <row r="119" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="11" t="s">
         <v>325</v>
       </c>
@@ -11553,8 +11898,11 @@
       <c r="Y119" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="120" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z119" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="120" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>326</v>
       </c>
@@ -11630,8 +11978,11 @@
       <c r="Y120" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="121" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z120" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="121" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="11" t="s">
         <v>327</v>
       </c>
@@ -11707,8 +12058,11 @@
       <c r="Y121" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="122" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z121" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="122" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>328</v>
       </c>
@@ -11724,7 +12078,7 @@
       <c r="E122" s="13">
         <v>55</v>
       </c>
-      <c r="F122" s="10" t="s">
+      <c r="F122" s="47" t="s">
         <v>183</v>
       </c>
       <c r="G122" s="19">
@@ -11784,8 +12138,11 @@
       <c r="Y122" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="123" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z122" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="123" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="11" t="s">
         <v>329</v>
       </c>
@@ -11801,7 +12158,7 @@
       <c r="E123" s="14">
         <v>56</v>
       </c>
-      <c r="F123" s="23" t="s">
+      <c r="F123" s="48" t="s">
         <v>183</v>
       </c>
       <c r="G123" s="20">
@@ -11861,8 +12218,11 @@
       <c r="Y123" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="124" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z123" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="124" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>330</v>
       </c>
@@ -11938,8 +12298,11 @@
       <c r="Y124" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="125" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z124" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="125" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="11" t="s">
         <v>331</v>
       </c>
@@ -12015,8 +12378,11 @@
       <c r="Y125" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="126" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z125" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="126" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>332</v>
       </c>
@@ -12092,8 +12458,11 @@
       <c r="Y126" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="127" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z126" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="127" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="11" t="s">
         <v>333</v>
       </c>
@@ -12169,8 +12538,11 @@
       <c r="Y127" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="128" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z127" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="128" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>334</v>
       </c>
@@ -12186,7 +12558,7 @@
       <c r="E128" s="13">
         <v>56</v>
       </c>
-      <c r="F128" s="10" t="s">
+      <c r="F128" s="47" t="s">
         <v>183</v>
       </c>
       <c r="G128" s="19">
@@ -12237,8 +12609,11 @@
       <c r="Y128" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="129" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z128" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="129" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="11" t="s">
         <v>335</v>
       </c>
@@ -12314,8 +12689,11 @@
       <c r="Y129" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="130" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z129" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="130" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>336</v>
       </c>
@@ -12391,8 +12769,11 @@
       <c r="Y130" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="131" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z130" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="131" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="11" t="s">
         <v>337</v>
       </c>
@@ -12408,7 +12789,7 @@
       <c r="E131" s="14">
         <v>54</v>
       </c>
-      <c r="F131" s="23" t="s">
+      <c r="F131" s="48" t="s">
         <v>183</v>
       </c>
       <c r="G131" s="20">
@@ -12459,8 +12840,11 @@
       <c r="Y131" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="132" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z131" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="132" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>338</v>
       </c>
@@ -12536,8 +12920,11 @@
       <c r="Y132" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="133" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z132" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="133" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="32" t="s">
         <v>339</v>
       </c>
@@ -12571,8 +12958,9 @@
       <c r="W133" s="41"/>
       <c r="X133" s="41"/>
       <c r="Y133" s="46"/>
-    </row>
-    <row r="134" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z133" s="46"/>
+    </row>
+    <row r="134" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>340</v>
       </c>
@@ -12648,8 +13036,11 @@
       <c r="Y134" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="135" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z134" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="135" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="11" t="s">
         <v>341</v>
       </c>
@@ -12725,8 +13116,11 @@
       <c r="Y135" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="136" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z135" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="136" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>342</v>
       </c>
@@ -12802,8 +13196,11 @@
       <c r="Y136" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="137" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z136" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="137" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="11" t="s">
         <v>343</v>
       </c>
@@ -12879,8 +13276,11 @@
       <c r="Y137" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="138" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z137" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="138" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>344</v>
       </c>
@@ -12956,8 +13356,11 @@
       <c r="Y138" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="139" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z138" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="139" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="11" t="s">
         <v>345</v>
       </c>
@@ -12973,7 +13376,7 @@
       <c r="E139" s="25">
         <v>56</v>
       </c>
-      <c r="F139" s="10" t="s">
+      <c r="F139" s="47" t="s">
         <v>183</v>
       </c>
       <c r="G139" s="20">
@@ -13033,8 +13436,11 @@
       <c r="Y139" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="140" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z139" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="140" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>346</v>
       </c>
@@ -13050,7 +13456,7 @@
       <c r="E140" s="14">
         <v>58</v>
       </c>
-      <c r="F140" s="10" t="s">
+      <c r="F140" s="47" t="s">
         <v>183</v>
       </c>
       <c r="G140" s="19">
@@ -13110,8 +13516,11 @@
       <c r="Y140" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="141" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z140" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="141" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="11" t="s">
         <v>347</v>
       </c>
@@ -13187,8 +13596,11 @@
       <c r="Y141" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="142" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z141" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="142" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>348</v>
       </c>
@@ -13204,7 +13616,7 @@
       <c r="E142" s="14">
         <v>54</v>
       </c>
-      <c r="F142" s="10" t="s">
+      <c r="F142" s="47" t="s">
         <v>183</v>
       </c>
       <c r="G142" s="19">
@@ -13264,8 +13676,11 @@
       <c r="Y142" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="143" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z142" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="143" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="11" t="s">
         <v>349</v>
       </c>
@@ -13341,8 +13756,11 @@
       <c r="Y143" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="144" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z143" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="144" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>350</v>
       </c>
@@ -13418,8 +13836,11 @@
       <c r="Y144" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="145" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z144" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="145" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="11" t="s">
         <v>351</v>
       </c>
@@ -13495,8 +13916,11 @@
       <c r="Y145" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="146" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z145" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="146" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>352</v>
       </c>
@@ -13572,8 +13996,11 @@
       <c r="Y146" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="147" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z146" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="147" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="11" t="s">
         <v>353</v>
       </c>
@@ -13649,8 +14076,11 @@
       <c r="Y147" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="148" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z147" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="148" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>354</v>
       </c>
@@ -13726,8 +14156,11 @@
       <c r="Y148" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="149" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z148" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="149" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="11" t="s">
         <v>355</v>
       </c>
@@ -13803,8 +14236,11 @@
       <c r="Y149" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="150" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z149" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="150" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>356</v>
       </c>
@@ -13880,8 +14316,11 @@
       <c r="Y150" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="151" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z150" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="151" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="11" t="s">
         <v>357</v>
       </c>
@@ -13957,8 +14396,11 @@
       <c r="Y151" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="152" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z151" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="152" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="26" t="s">
         <v>358</v>
       </c>
@@ -13992,8 +14434,9 @@
       <c r="W152" s="41"/>
       <c r="X152" s="41"/>
       <c r="Y152" s="46"/>
-    </row>
-    <row r="153" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z152" s="46"/>
+    </row>
+    <row r="153" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>568</v>
       </c>
@@ -14069,8 +14512,11 @@
       <c r="Y153" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="154" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z153" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="154" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="11" t="s">
         <v>359</v>
       </c>
@@ -14146,8 +14592,11 @@
       <c r="Y154" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="155" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z154" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="155" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="9" t="s">
         <v>360</v>
       </c>
@@ -14223,8 +14672,11 @@
       <c r="Y155" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="156" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z155" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="156" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="11" t="s">
         <v>361</v>
       </c>
@@ -14300,8 +14752,11 @@
       <c r="Y156" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="157" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z156" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="157" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="9" t="s">
         <v>362</v>
       </c>
@@ -14377,8 +14832,11 @@
       <c r="Y157" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="158" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z157" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="158" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="11" t="s">
         <v>363</v>
       </c>
@@ -14454,8 +14912,11 @@
       <c r="Y158" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="159" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z158" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="159" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="9" t="s">
         <v>364</v>
       </c>
@@ -14531,8 +14992,11 @@
       <c r="Y159" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="160" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z159" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="160" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="11" t="s">
         <v>365</v>
       </c>
@@ -14608,8 +15072,11 @@
       <c r="Y160" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="161" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z160" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="161" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="9" t="s">
         <v>366</v>
       </c>
@@ -14685,8 +15152,11 @@
       <c r="Y161" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="162" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z161" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="162" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="11" t="s">
         <v>367</v>
       </c>
@@ -14762,8 +15232,11 @@
       <c r="Y162" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="163" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z162" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="163" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="9" t="s">
         <v>368</v>
       </c>
@@ -14839,8 +15312,11 @@
       <c r="Y163" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="164" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z163" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="164" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="11" t="s">
         <v>369</v>
       </c>
@@ -14916,8 +15392,11 @@
       <c r="Y164" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="165" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z164" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="165" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="9" t="s">
         <v>370</v>
       </c>
@@ -14993,8 +15472,11 @@
       <c r="Y165" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="166" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z165" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="166" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="11" t="s">
         <v>371</v>
       </c>
@@ -15070,8 +15552,11 @@
       <c r="Y166" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="167" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z166" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="167" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="9" t="s">
         <v>372</v>
       </c>
@@ -15147,8 +15632,11 @@
       <c r="Y167" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="168" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z167" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="168" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="11" t="s">
         <v>373</v>
       </c>
@@ -15224,8 +15712,11 @@
       <c r="Y168" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="169" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z168" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="169" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="9" t="s">
         <v>374</v>
       </c>
@@ -15301,8 +15792,11 @@
       <c r="Y169" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="170" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z169" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="170" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="11" t="s">
         <v>375</v>
       </c>
@@ -15378,8 +15872,11 @@
       <c r="Y170" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="171" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z170" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="171" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="9" t="s">
         <v>376</v>
       </c>
@@ -15455,8 +15952,11 @@
       <c r="Y171" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="172" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z171" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="172" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="11" t="s">
         <v>377</v>
       </c>
@@ -15532,8 +16032,11 @@
       <c r="Y172" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="173" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z172" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="173" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="9" t="s">
         <v>378</v>
       </c>
@@ -15609,8 +16112,11 @@
       <c r="Y173" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="174" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z173" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="174" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="11" t="s">
         <v>379</v>
       </c>
@@ -15686,8 +16192,11 @@
       <c r="Y174" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="175" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z174" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="175" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="9" t="s">
         <v>380</v>
       </c>
@@ -15763,8 +16272,11 @@
       <c r="Y175" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="176" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z175" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="176" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="11" t="s">
         <v>381</v>
       </c>
@@ -15840,12 +16352,15 @@
       <c r="Y176" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="177" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z176" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="177" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="9" t="s">
         <v>382</v>
       </c>
-      <c r="B177" s="15" t="s">
+      <c r="B177" s="43" t="s">
         <v>78</v>
       </c>
       <c r="C177" s="2" t="s">
@@ -15857,7 +16372,7 @@
       <c r="E177" s="13">
         <v>59</v>
       </c>
-      <c r="F177" s="10" t="s">
+      <c r="F177" s="47" t="s">
         <v>183</v>
       </c>
       <c r="G177" s="19">
@@ -15917,8 +16432,11 @@
       <c r="Y177" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="178" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z177" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="178" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="11" t="s">
         <v>383</v>
       </c>
@@ -15994,8 +16512,11 @@
       <c r="Y178" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="179" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z178" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="179" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="9" t="s">
         <v>384</v>
       </c>
@@ -16071,8 +16592,11 @@
       <c r="Y179" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="180" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z179" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="180" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="11" t="s">
         <v>385</v>
       </c>
@@ -16148,8 +16672,11 @@
       <c r="Y180" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="181" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z180" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="181" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="9" t="s">
         <v>386</v>
       </c>
@@ -16225,8 +16752,11 @@
       <c r="Y181" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="182" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z181" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="182" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="11" t="s">
         <v>387</v>
       </c>
@@ -16302,8 +16832,11 @@
       <c r="Y182" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="183" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z182" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="183" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="9" t="s">
         <v>388</v>
       </c>
@@ -16379,8 +16912,11 @@
       <c r="Y183" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="184" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z183" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="184" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="11" t="s">
         <v>389</v>
       </c>
@@ -16456,8 +16992,11 @@
       <c r="Y184" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="185" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z184" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="185" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="9" t="s">
         <v>390</v>
       </c>
@@ -16533,8 +17072,11 @@
       <c r="Y185" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="186" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z185" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="186" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="11" t="s">
         <v>391</v>
       </c>
@@ -16610,8 +17152,11 @@
       <c r="Y186" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="187" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z186" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="187" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="9" t="s">
         <v>392</v>
       </c>
@@ -16687,8 +17232,11 @@
       <c r="Y187" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="188" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z187" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="188" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="11" t="s">
         <v>393</v>
       </c>
@@ -16764,8 +17312,11 @@
       <c r="Y188" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="189" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z188" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="189" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="9" t="s">
         <v>394</v>
       </c>
@@ -16841,8 +17392,11 @@
       <c r="Y189" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="190" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z189" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="190" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="11" t="s">
         <v>395</v>
       </c>
@@ -16918,8 +17472,11 @@
       <c r="Y190" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="191" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z190" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="191" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="9" t="s">
         <v>396</v>
       </c>
@@ -16995,8 +17552,11 @@
       <c r="Y191" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="192" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z191" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="192" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="11" t="s">
         <v>397</v>
       </c>
@@ -17072,8 +17632,11 @@
       <c r="Y192" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="193" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z192" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="193" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="9" t="s">
         <v>398</v>
       </c>
@@ -17149,8 +17712,11 @@
       <c r="Y193" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="194" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z193" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="194" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="11" t="s">
         <v>399</v>
       </c>
@@ -17226,8 +17792,11 @@
       <c r="Y194" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="195" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z194" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="195" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A195" s="9" t="s">
         <v>400</v>
       </c>
@@ -17303,8 +17872,11 @@
       <c r="Y195" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="196" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z195" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="196" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A196" s="11" t="s">
         <v>401</v>
       </c>
@@ -17380,8 +17952,11 @@
       <c r="Y196" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="197" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z196" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="197" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A197" s="9" t="s">
         <v>402</v>
       </c>
@@ -17457,8 +18032,11 @@
       <c r="Y197" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="198" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z197" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="198" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A198" s="11" t="s">
         <v>403</v>
       </c>
@@ -17534,8 +18112,11 @@
       <c r="Y198" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="199" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z198" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="199" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A199" s="9" t="s">
         <v>404</v>
       </c>
@@ -17611,8 +18192,11 @@
       <c r="Y199" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="200" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z199" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="200" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A200" s="11" t="s">
         <v>405</v>
       </c>
@@ -17688,8 +18272,11 @@
       <c r="Y200" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="201" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z200" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="201" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A201" s="9" t="s">
         <v>406</v>
       </c>
@@ -17765,8 +18352,11 @@
       <c r="Y201" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="202" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z201" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="202" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A202" s="11" t="s">
         <v>407</v>
       </c>
@@ -17842,8 +18432,11 @@
       <c r="Y202" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="203" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z202" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="203" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A203" s="9" t="s">
         <v>408</v>
       </c>
@@ -17919,8 +18512,11 @@
       <c r="Y203" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="204" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z203" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="204" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A204" s="11" t="s">
         <v>409</v>
       </c>
@@ -17996,8 +18592,11 @@
       <c r="Y204" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="205" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z204" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="205" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="9" t="s">
         <v>410</v>
       </c>
@@ -18073,8 +18672,11 @@
       <c r="Y205" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="206" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z205" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="206" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="11" t="s">
         <v>411</v>
       </c>
@@ -18150,8 +18752,11 @@
       <c r="Y206" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="207" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z206" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="207" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A207" s="9" t="s">
         <v>412</v>
       </c>
@@ -18227,8 +18832,11 @@
       <c r="Y207" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="208" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z207" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="208" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A208" s="11" t="s">
         <v>413</v>
       </c>
@@ -18304,8 +18912,11 @@
       <c r="Y208" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="209" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z208" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="209" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A209" s="9" t="s">
         <v>414</v>
       </c>
@@ -18381,8 +18992,11 @@
       <c r="Y209" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="210" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z209" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="210" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="11" t="s">
         <v>415</v>
       </c>
@@ -18458,8 +19072,11 @@
       <c r="Y210" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="211" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z210" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="211" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="9" t="s">
         <v>416</v>
       </c>
@@ -18535,8 +19152,11 @@
       <c r="Y211" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="212" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z211" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="212" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A212" s="11" t="s">
         <v>417</v>
       </c>
@@ -18612,8 +19232,11 @@
       <c r="Y212" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="213" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z212" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="213" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A213" s="9" t="s">
         <v>418</v>
       </c>
@@ -18689,8 +19312,11 @@
       <c r="Y213" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="214" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z213" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="214" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A214" s="11" t="s">
         <v>419</v>
       </c>
@@ -18766,8 +19392,11 @@
       <c r="Y214" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="215" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z214" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="215" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A215" s="9" t="s">
         <v>420</v>
       </c>
@@ -18843,8 +19472,11 @@
       <c r="Y215" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="216" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z215" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="216" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A216" s="11" t="s">
         <v>421</v>
       </c>
@@ -18920,8 +19552,11 @@
       <c r="Y216" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="217" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z216" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="217" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A217" s="9" t="s">
         <v>422</v>
       </c>
@@ -18997,8 +19632,11 @@
       <c r="Y217" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="218" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z217" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="218" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="11" t="s">
         <v>423</v>
       </c>
@@ -19074,8 +19712,11 @@
       <c r="Y218" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="219" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z218" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="219" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A219" s="9" t="s">
         <v>424</v>
       </c>
@@ -19151,8 +19792,11 @@
       <c r="Y219" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="220" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z219" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="220" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A220" s="11" t="s">
         <v>425</v>
       </c>
@@ -19228,8 +19872,11 @@
       <c r="Y220" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="221" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z220" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="221" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="9" t="s">
         <v>426</v>
       </c>
@@ -19305,8 +19952,11 @@
       <c r="Y221" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="222" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z221" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="222" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A222" s="11" t="s">
         <v>427</v>
       </c>
@@ -19382,8 +20032,11 @@
       <c r="Y222" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="223" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z222" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="223" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="9" t="s">
         <v>428</v>
       </c>
@@ -19459,8 +20112,11 @@
       <c r="Y223" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="224" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z223" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="224" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A224" s="11" t="s">
         <v>429</v>
       </c>
@@ -19536,8 +20192,11 @@
       <c r="Y224" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="225" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z224" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="225" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A225" s="9" t="s">
         <v>430</v>
       </c>
@@ -19613,8 +20272,11 @@
       <c r="Y225" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="226" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z225" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="226" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A226" s="11" t="s">
         <v>431</v>
       </c>
@@ -19690,8 +20352,11 @@
       <c r="Y226" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="227" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z226" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="227" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="9" t="s">
         <v>432</v>
       </c>
@@ -19767,8 +20432,11 @@
       <c r="Y227" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="228" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z227" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="228" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="11" t="s">
         <v>433</v>
       </c>
@@ -19844,8 +20512,11 @@
       <c r="Y228" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="229" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z228" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="229" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A229" s="9" t="s">
         <v>434</v>
       </c>
@@ -19921,8 +20592,11 @@
       <c r="Y229" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="230" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z229" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="230" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="11" t="s">
         <v>435</v>
       </c>
@@ -19998,8 +20672,11 @@
       <c r="Y230" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="231" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z230" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="231" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A231" s="9" t="s">
         <v>436</v>
       </c>
@@ -20075,8 +20752,11 @@
       <c r="Y231" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="232" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z231" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="232" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A232" s="11" t="s">
         <v>437</v>
       </c>
@@ -20152,8 +20832,11 @@
       <c r="Y232" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="233" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z232" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="233" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A233" s="9" t="s">
         <v>438</v>
       </c>
@@ -20229,8 +20912,11 @@
       <c r="Y233" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="234" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z233" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="234" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A234" s="11" t="s">
         <v>439</v>
       </c>
@@ -20306,8 +20992,11 @@
       <c r="Y234" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="235" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z234" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="235" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A235" s="9" t="s">
         <v>440</v>
       </c>
@@ -20383,8 +21072,11 @@
       <c r="Y235" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="236" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z235" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="236" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A236" s="11" t="s">
         <v>441</v>
       </c>
@@ -20460,8 +21152,11 @@
       <c r="Y236" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="237" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z236" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="237" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A237" s="9" t="s">
         <v>442</v>
       </c>
@@ -20537,8 +21232,11 @@
       <c r="Y237" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="238" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z237" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="238" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A238" s="11" t="s">
         <v>443</v>
       </c>
@@ -20614,8 +21312,11 @@
       <c r="Y238" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="239" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z238" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="239" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A239" s="9" t="s">
         <v>444</v>
       </c>
@@ -20691,8 +21392,11 @@
       <c r="Y239" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="240" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z239" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="240" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A240" s="11" t="s">
         <v>445</v>
       </c>
@@ -20768,8 +21472,11 @@
       <c r="Y240" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="241" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z240" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="241" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A241" s="9" t="s">
         <v>446</v>
       </c>
@@ -20845,8 +21552,11 @@
       <c r="Y241" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="242" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z241" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="242" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A242" s="11" t="s">
         <v>447</v>
       </c>
@@ -20922,8 +21632,11 @@
       <c r="Y242" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="243" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z242" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="243" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="9" t="s">
         <v>448</v>
       </c>
@@ -20999,8 +21712,11 @@
       <c r="Y243" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="244" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z243" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="244" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="11" t="s">
         <v>449</v>
       </c>
@@ -21076,8 +21792,11 @@
       <c r="Y244" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="245" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z244" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="245" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="9" t="s">
         <v>450</v>
       </c>
@@ -21153,8 +21872,11 @@
       <c r="Y245" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="246" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z245" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="246" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A246" s="11" t="s">
         <v>451</v>
       </c>
@@ -21230,8 +21952,11 @@
       <c r="Y246" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="247" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z246" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="247" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A247" s="9" t="s">
         <v>452</v>
       </c>
@@ -21307,8 +22032,11 @@
       <c r="Y247" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="248" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z247" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="248" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="11" t="s">
         <v>453</v>
       </c>
@@ -21384,8 +22112,11 @@
       <c r="Y248" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="249" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z248" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="249" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="9" t="s">
         <v>454</v>
       </c>
@@ -21461,8 +22192,11 @@
       <c r="Y249" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="250" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z249" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="250" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="11" t="s">
         <v>455</v>
       </c>
@@ -21538,8 +22272,11 @@
       <c r="Y250" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="251" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z250" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="251" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="9" t="s">
         <v>456</v>
       </c>
@@ -21615,8 +22352,11 @@
       <c r="Y251" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="252" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z251" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="252" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="11" t="s">
         <v>457</v>
       </c>
@@ -21692,8 +22432,11 @@
       <c r="Y252" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="253" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z252" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="253" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="9" t="s">
         <v>458</v>
       </c>
@@ -21769,8 +22512,11 @@
       <c r="Y253" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="254" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z253" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="254" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="11" t="s">
         <v>459</v>
       </c>
@@ -21846,8 +22592,11 @@
       <c r="Y254" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="255" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z254" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="255" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="9" t="s">
         <v>460</v>
       </c>
@@ -21923,8 +22672,11 @@
       <c r="Y255" s="46">
         <v>44443</v>
       </c>
-    </row>
-    <row r="256" spans="1:25" ht="23.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z255" s="46">
+        <v>44444</v>
+      </c>
+    </row>
+    <row r="256" spans="1:26" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="11" t="s">
         <v>461</v>
       </c>
@@ -21999,6 +22751,9 @@
       </c>
       <c r="Y256" s="46">
         <v>44443</v>
+      </c>
+      <c r="Z256" s="46">
+        <v>44444</v>
       </c>
     </row>
     <row r="257" spans="1:16" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -26790,11 +27545,6 @@
       <c r="L536" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z256" xr:uid="{0593BD49-364B-49CF-AB09-840279B88535}">
-    <filterColumn colId="3">
-      <colorFilter dxfId="0"/>
-    </filterColumn>
-  </autoFilter>
   <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.43307086614173229" right="0.11811023622047245" top="0.51181102362204722" bottom="0.19685039370078741" header="0.19685039370078741" footer="0.11811023622047245"/>

</xml_diff>

<commit_message>
kirim sepatu taruna 2021 05 sept
</commit_message>
<xml_diff>
--- a/27. TARUNA 2021-2 E(K_1) N(K_2) T(K_3)/UKURAN.xlsx
+++ b/27. TARUNA 2021-2 E(K_1) N(K_2) T(K_3)/UKURAN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mapan\progress\27. TARUNA 2021-2 E(K_1) N(K_2) T(K_3)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7F3F19-15D5-442E-B15E-ACD010F8C482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABFC64A-58BA-4E08-8046-D53924682B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D0EA34A-D090-461B-B73E-10F00D55D97B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1332" uniqueCount="571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="572">
   <si>
     <t>ARUM PAMBUDININGTYAS</t>
   </si>
@@ -1744,6 +1744,9 @@
   </si>
   <si>
     <t>28 agust</t>
+  </si>
+  <si>
+    <t>kirim 05 sept</t>
   </si>
 </sst>
 </file>
@@ -2404,8 +2407,8 @@
   <dimension ref="A1:Z536"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E121" sqref="E121"/>
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -27557,15 +27560,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F0D2B3-E601-4F53-A109-AB1348321EE0}">
-  <dimension ref="B2:L12"/>
+  <dimension ref="B2:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>563</v>
       </c>
@@ -27590,8 +27593,11 @@
       <c r="L2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="17">
         <v>53</v>
       </c>
@@ -27621,7 +27627,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="14">
         <v>54</v>
       </c>
@@ -27650,8 +27656,11 @@
         <f>COUNTIFS(SEMUA!$F$1:$F$256,rekap!$L$2,SEMUA!$D$1:$D$256,rekap!J4)</f>
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="13">
         <v>55</v>
       </c>
@@ -27680,8 +27689,11 @@
         <f>COUNTIFS(SEMUA!$F$1:$F$256,rekap!$L$2,SEMUA!$D$1:$D$256,rekap!J5)</f>
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="14">
         <v>56</v>
       </c>
@@ -27710,8 +27722,11 @@
         <f>COUNTIFS(SEMUA!$F$1:$F$256,rekap!$L$2,SEMUA!$D$1:$D$256,rekap!J6)</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="13">
         <v>57</v>
       </c>
@@ -27740,8 +27755,11 @@
         <f>COUNTIFS(SEMUA!$F$1:$F$256,rekap!$L$2,SEMUA!$D$1:$D$256,rekap!J7)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="14">
         <v>58</v>
       </c>
@@ -27770,8 +27788,11 @@
         <f>COUNTIFS(SEMUA!$F$1:$F$256,rekap!$L$2,SEMUA!$D$1:$D$256,rekap!J8)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="13">
         <v>59</v>
       </c>
@@ -27800,8 +27821,11 @@
         <f>COUNTIFS(SEMUA!$F$1:$F$256,rekap!$L$2,SEMUA!$D$1:$D$256,rekap!J9)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="14">
         <v>60</v>
       </c>
@@ -27830,8 +27854,11 @@
         <f>COUNTIFS(SEMUA!$F$1:$F$256,rekap!$L$2,SEMUA!$D$1:$D$256,rekap!J10)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="13"/>
       <c r="C11">
         <f>SUM(C3:C10)</f>
@@ -27861,7 +27888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="K12">
         <f>SUM(K3:K11)</f>
         <v>224</v>
@@ -27869,6 +27896,10 @@
       <c r="L12">
         <f>SUM(L3:L11)</f>
         <v>28</v>
+      </c>
+      <c r="M12">
+        <f>SUM(M3:M11)</f>
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>